<commit_message>
upload url of tableau with data vizualization
</commit_message>
<xml_diff>
--- a/Tableau Vizualization/Tableau Table 3.xlsx
+++ b/Tableau Vizualization/Tableau Table 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esposito\workspace\Datos\Data-Analyst-Portfolio-Project-Repository\Tableau Vizualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D6EF830-1E43-4F9E-837E-8FCFC1110691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AB8CAC-FC09-4C2F-9873-A25F1019D207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{82EE9232-A76F-4704-BB26-0E78CD802352}"/>
   </bookViews>
@@ -711,7 +711,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,6 +721,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -745,16 +752,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1069,13 +1078,14 @@
   <dimension ref="A1:D220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,7 +1098,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1102,7 +1112,7 @@
       <c r="C2">
         <v>33374.536</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>4125.4061804697203</v>
       </c>
     </row>
@@ -1116,7 +1126,7 @@
       <c r="C3">
         <v>149272.20199999999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>439.83794566562602</v>
       </c>
     </row>
@@ -1130,7 +1140,7 @@
       <c r="C4">
         <v>171254.77299999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>221.64598848120099</v>
       </c>
     </row>
@@ -1144,7 +1154,7 @@
       <c r="C5">
         <v>76723.392000000007</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>201.17836222041601</v>
       </c>
     </row>
@@ -1158,7 +1168,7 @@
       <c r="C6">
         <v>62531.851999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>159.34117826929</v>
       </c>
     </row>
@@ -1172,7 +1182,7 @@
       <c r="C7">
         <v>59721.375</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>60.729484441732801</v>
       </c>
     </row>
@@ -1186,7 +1196,7 @@
       <c r="C8">
         <v>155062.717</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>24.689077989115699</v>
       </c>
     </row>
@@ -1200,7 +1210,7 @@
       <c r="C9">
         <v>107360.34600000001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>17.150872557414299</v>
       </c>
     </row>
@@ -1214,7 +1224,7 @@
       <c r="C10">
         <v>68605.490999999995</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>15.537810023576601</v>
       </c>
     </row>
@@ -1242,7 +1252,7 @@
       <c r="C12">
         <v>24789.113000000001</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>13.4995632498135</v>
       </c>
     </row>
@@ -1256,7 +1266,7 @@
       <c r="C13">
         <v>12580.672</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>12.846858916755201</v>
       </c>
     </row>
@@ -1270,7 +1280,7 @@
       <c r="C14">
         <v>55194.601000000002</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>10.2109736153712</v>
       </c>
     </row>
@@ -1284,7 +1294,7 @@
       <c r="C15">
         <v>74475.482000000004</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>8.5027476912292403</v>
       </c>
     </row>
@@ -1298,7 +1308,7 @@
       <c r="C16">
         <v>31859.484</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>8.0125254953837892</v>
       </c>
     </row>
@@ -1312,7 +1322,7 @@
       <c r="C17">
         <v>42954.163999999997</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>7.7257358072476396</v>
       </c>
     </row>
@@ -1326,7 +1336,7 @@
       <c r="C18">
         <v>91982.971999999994</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>6.9340571215772799</v>
       </c>
     </row>
@@ -1340,7 +1350,7 @@
       <c r="C19">
         <v>26581.19</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>6.7593961062738996</v>
       </c>
     </row>
@@ -1354,7 +1364,7 @@
       <c r="C20">
         <v>103981.99800000001</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>6.1108977934076698</v>
       </c>
     </row>
@@ -1368,7 +1378,7 @@
       <c r="C21">
         <v>115584.348</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>5.55979454835464</v>
       </c>
     </row>
@@ -1382,7 +1392,7 @@
       <c r="C22">
         <v>18965.567999999999</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>5.5576756043955999</v>
       </c>
     </row>
@@ -1396,7 +1406,7 @@
       <c r="C23">
         <v>10503.694</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>4.7926839173028002</v>
       </c>
     </row>
@@ -1410,7 +1420,7 @@
       <c r="C24">
         <v>13414.715</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>4.6680823743523199</v>
       </c>
     </row>
@@ -1424,7 +1434,7 @@
       <c r="C25">
         <v>73134.521999999997</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>3.51037842352331</v>
       </c>
     </row>
@@ -1438,7 +1448,7 @@
       <c r="C26">
         <v>2416.9690000000001</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>3.3573210540206402</v>
       </c>
     </row>
@@ -1452,7 +1462,7 @@
       <c r="C27">
         <v>90831.214999999997</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>3.3365725780234401</v>
       </c>
     </row>
@@ -1466,7 +1476,7 @@
       <c r="C28">
         <v>62855.41</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>3.3323795648610299</v>
       </c>
     </row>
@@ -1480,7 +1490,7 @@
       <c r="C29">
         <v>17665.187999999998</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>3.0112792644135902</v>
       </c>
     </row>
@@ -1494,7 +1504,7 @@
       <c r="C30">
         <v>53621.375</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>2.7743220366168</v>
       </c>
     </row>
@@ -1508,7 +1518,7 @@
       <c r="C31">
         <v>71380.672000000006</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>2.47758366712252</v>
       </c>
     </row>
@@ -1522,7 +1532,7 @@
       <c r="C32">
         <v>72914.929999999993</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>2.4606537991937198</v>
       </c>
     </row>
@@ -1536,7 +1546,7 @@
       <c r="C33">
         <v>16887.481</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>2.1470075353533602</v>
       </c>
     </row>
@@ -1550,7 +1560,7 @@
       <c r="C34">
         <v>80916.275999999998</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>1.9710351674969799</v>
       </c>
     </row>
@@ -1564,7 +1574,7 @@
       <c r="C35">
         <v>84494.925000000003</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>1.95827272752556</v>
       </c>
     </row>
@@ -1578,7 +1588,7 @@
       <c r="C36">
         <v>77788.013999999996</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>1.9499774765458999</v>
       </c>
     </row>
@@ -1592,7 +1602,7 @@
       <c r="C37">
         <v>60491.372000000003</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>1.84379100924618</v>
       </c>
     </row>
@@ -1606,7 +1616,7 @@
       <c r="C38">
         <v>57122.508000000002</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>1.6444155801535401</v>
       </c>
     </row>
@@ -1620,7 +1630,7 @@
       <c r="C39">
         <v>45550.42</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>1.5828209048578801</v>
       </c>
     </row>
@@ -1634,7 +1644,7 @@
       <c r="C40">
         <v>827.19200000000001</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>1.5551060309821001</v>
       </c>
     </row>
@@ -1648,7 +1658,7 @@
       <c r="C41">
         <v>62181.284</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>1.54144408364678</v>
       </c>
     </row>
@@ -1662,7 +1672,7 @@
       <c r="C42">
         <v>64158.050999999999</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>1.5023323856831099</v>
       </c>
     </row>
@@ -1676,7 +1686,7 @@
       <c r="C43">
         <v>101336.94899999999</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>1.4892426971417601</v>
       </c>
     </row>
@@ -1690,7 +1700,7 @@
       <c r="C44">
         <v>152279.46</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>1.42197885849467</v>
       </c>
     </row>
@@ -1704,7 +1714,7 @@
       <c r="C45">
         <v>15909.82</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>1.3713423274640499</v>
       </c>
     </row>
@@ -1718,7 +1728,7 @@
       <c r="C46">
         <v>70006.592000000004</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>1.2822558544578799</v>
       </c>
     </row>
@@ -1732,7 +1742,7 @@
       <c r="C47">
         <v>1421.982</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>1.2637705631937699</v>
       </c>
     </row>
@@ -1746,7 +1756,7 @@
       <c r="C48">
         <v>58113.669000000002</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>1.1391674193988499</v>
       </c>
     </row>
@@ -1760,7 +1770,7 @@
       <c r="C49">
         <v>11234.795</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>1.13712269813219</v>
       </c>
     </row>
@@ -1774,7 +1784,7 @@
       <c r="C50">
         <v>77149.289000000004</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>1.13031931118893</v>
       </c>
     </row>
@@ -1788,7 +1798,7 @@
       <c r="C51">
         <v>96872.164999999994</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>1.1191924918384699</v>
       </c>
     </row>
@@ -1802,7 +1812,7 @@
       <c r="C52">
         <v>50401.029000000002</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>1.0207191427106299</v>
       </c>
     </row>
@@ -1816,7 +1826,7 @@
       <c r="C53">
         <v>49270.786</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>0.96721011740216301</v>
       </c>
     </row>
@@ -1830,7 +1840,7 @@
       <c r="C54">
         <v>96403.403000000006</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>0.95455813142930102</v>
       </c>
     </row>
@@ -1844,7 +1854,7 @@
       <c r="C55">
         <v>76256.861000000004</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="1">
         <v>0.88111180643674902</v>
       </c>
     </row>
@@ -1858,7 +1868,7 @@
       <c r="C56">
         <v>19958.114000000001</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="1">
         <v>0.84869458353266403</v>
       </c>
     </row>
@@ -1872,7 +1882,7 @@
       <c r="C57">
         <v>58197.194000000003</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>0.83755709370945597</v>
       </c>
     </row>
@@ -1886,7 +1896,7 @@
       <c r="C58">
         <v>80674.923999999999</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="1">
         <v>0.835113883037364</v>
       </c>
     </row>
@@ -1900,7 +1910,7 @@
       <c r="C59">
         <v>82035.601999999999</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="1">
         <v>0.804530344943716</v>
       </c>
     </row>
@@ -1914,7 +1924,7 @@
       <c r="C60">
         <v>68714.47</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="1">
         <v>0.76295156777402695</v>
       </c>
     </row>
@@ -1928,7 +1938,7 @@
       <c r="C61">
         <v>19028.964</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="1">
         <v>0.74890173465002396</v>
       </c>
     </row>
@@ -1942,7 +1952,7 @@
       <c r="C62">
         <v>43377.105000000003</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="1">
         <v>0.74888785838479799</v>
       </c>
     </row>
@@ -1956,7 +1966,7 @@
       <c r="C63">
         <v>37843.608</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="1">
         <v>0.74106930178109898</v>
       </c>
     </row>
@@ -1970,7 +1980,7 @@
       <c r="C64">
         <v>85441.053</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="1">
         <v>0.73722074139471105</v>
       </c>
     </row>
@@ -1984,7 +1994,7 @@
       <c r="C65">
         <v>69720.987999999998</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="1">
         <v>0.68332873997612498</v>
       </c>
     </row>
@@ -1998,7 +2008,7 @@
       <c r="C66">
         <v>7734.241</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
         <v>0.552646712268961</v>
       </c>
     </row>
@@ -2012,7 +2022,7 @@
       <c r="C67">
         <v>39127.35</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="1">
         <v>0.548576031225946</v>
       </c>
     </row>
@@ -2026,7 +2036,7 @@
       <c r="C68">
         <v>52600.097000000002</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
         <v>0.53182982488069197</v>
       </c>
     </row>
@@ -2040,7 +2050,7 @@
       <c r="C69">
         <v>15391.936</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="1">
         <v>0.51979395919370797</v>
       </c>
     </row>
@@ -2054,7 +2064,7 @@
       <c r="C70">
         <v>88881.486999999994</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="1">
         <v>0.51871692892033705</v>
       </c>
     </row>
@@ -2068,7 +2078,7 @@
       <c r="C71">
         <v>4408.9489999999996</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="1">
         <v>0.50701176984688301</v>
       </c>
     </row>
@@ -2082,7 +2092,7 @@
       <c r="C72">
         <v>10367.394</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="1">
         <v>0.46579788725306998</v>
       </c>
     </row>
@@ -2096,7 +2106,7 @@
       <c r="C73">
         <v>37964.421000000002</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="1">
         <v>0.40176877259223198</v>
       </c>
     </row>
@@ -2110,7 +2120,7 @@
       <c r="C74">
         <v>5484.0219999999999</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="1">
         <v>0.39088243994055499</v>
       </c>
     </row>
@@ -2124,7 +2134,7 @@
       <c r="C75">
         <v>20838.398000000001</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="1">
         <v>0.38438420568570802</v>
       </c>
     </row>
@@ -2138,7 +2148,7 @@
       <c r="C76">
         <v>25833.296999999999</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="1">
         <v>0.37596009306553502</v>
       </c>
     </row>
@@ -2152,7 +2162,7 @@
       <c r="C77">
         <v>11373.3</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="1">
         <v>0.34692760742484202</v>
       </c>
     </row>
@@ -2166,7 +2176,7 @@
       <c r="C78">
         <v>62682.146000000001</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="1">
         <v>0.32790050579589303</v>
       </c>
     </row>
@@ -2180,7 +2190,7 @@
       <c r="C79">
         <v>33102.862999999998</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="1">
         <v>0.317592681071655</v>
       </c>
     </row>
@@ -2194,7 +2204,7 @@
       <c r="C80">
         <v>31472.876</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <v>0.31040864764638099</v>
       </c>
     </row>
@@ -2208,7 +2218,7 @@
       <c r="C81">
         <v>54854.061999999998</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="1">
         <v>0.28513862532918499</v>
       </c>
     </row>
@@ -2222,7 +2232,7 @@
       <c r="C82">
         <v>15667.284</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="1">
         <v>0.28276631295799598</v>
       </c>
     </row>
@@ -2236,7 +2246,7 @@
       <c r="C83">
         <v>5009.2150000000001</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="1">
         <v>0.23382940008925199</v>
       </c>
     </row>
@@ -2250,7 +2260,7 @@
       <c r="C84">
         <v>24572.580999999998</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="1">
         <v>0.226519159830323</v>
       </c>
     </row>
@@ -2264,7 +2274,7 @@
       <c r="C85">
         <v>14603.343000000001</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="1">
         <v>0.223833774946196</v>
       </c>
     </row>
@@ -2278,7 +2288,7 @@
       <c r="C86">
         <v>26019.982</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>0.222906856480867</v>
       </c>
     </row>
@@ -2292,7 +2302,7 @@
       <c r="C87">
         <v>26155.258000000002</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="1">
         <v>0.22130555366118099</v>
       </c>
     </row>
@@ -2306,7 +2316,7 @@
       <c r="C88">
         <v>21437.798999999999</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="1">
         <v>0.21644268001318201</v>
       </c>
     </row>
@@ -2320,7 +2330,7 @@
       <c r="C89">
         <v>73775.23</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="1">
         <v>0.19493222707822799</v>
       </c>
     </row>
@@ -2334,7 +2344,7 @@
       <c r="C90">
         <v>1391.8910000000001</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="1">
         <v>0.18038742269430699</v>
       </c>
     </row>
@@ -2348,7 +2358,7 @@
       <c r="C91">
         <v>10451.523999999999</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="1">
         <v>0.17864805533624301</v>
       </c>
     </row>
@@ -2362,7 +2372,7 @@
       <c r="C92">
         <v>54575.197</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="1">
         <v>0.16552059899830901</v>
       </c>
     </row>
@@ -2376,7 +2386,7 @@
       <c r="C93">
         <v>10668.495000000001</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="1">
         <v>0.16447987042029699</v>
       </c>
     </row>
@@ -2390,7 +2400,7 @@
       <c r="C94">
         <v>75373.615000000005</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="1">
         <v>0.161210490486075</v>
       </c>
     </row>
@@ -2404,7 +2414,7 @@
       <c r="C95">
         <v>65877.017999999996</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="1">
         <v>0.14575923321331499</v>
       </c>
     </row>
@@ -2418,7 +2428,7 @@
       <c r="C96">
         <v>1726.28</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="1">
         <v>0.13093332888363701</v>
       </c>
     </row>
@@ -2432,7 +2442,7 @@
       <c r="C97">
         <v>21643.751</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="1">
         <v>0.122675720651633</v>
       </c>
     </row>
@@ -2446,7 +2456,7 @@
       <c r="C98">
         <v>83316.620999999999</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="1">
         <v>0.1222589124705</v>
       </c>
     </row>
@@ -2460,7 +2470,7 @@
       <c r="C99">
         <v>512.02</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="1">
         <v>0.117037690607406</v>
       </c>
     </row>
@@ -2474,7 +2484,7 @@
       <c r="C100">
         <v>67.573999999999998</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="1">
         <v>0.114156840220293</v>
       </c>
     </row>
@@ -2488,7 +2498,7 @@
       <c r="C101">
         <v>48568.201000000001</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="1">
         <v>0.11105425673562599</v>
       </c>
     </row>
@@ -2502,7 +2512,7 @@
       <c r="C102">
         <v>56202.082000000002</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="1">
         <v>0.110453806038195</v>
       </c>
     </row>
@@ -2516,7 +2526,7 @@
       <c r="C103">
         <v>66532.11</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="1">
         <v>0.110039858536861</v>
       </c>
     </row>
@@ -2530,7 +2540,7 @@
       <c r="C104">
         <v>20000.258999999998</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="1">
         <v>0.106516328981434</v>
       </c>
     </row>
@@ -2544,7 +2554,7 @@
       <c r="C105">
         <v>2440.5540000000001</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="1">
         <v>0.100988552814955</v>
       </c>
     </row>
@@ -2558,7 +2568,7 @@
       <c r="C106">
         <v>1897.36</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="1">
         <v>9.6410667084011303E-2</v>
       </c>
     </row>
@@ -2572,7 +2582,7 @@
       <c r="C107">
         <v>65289.54</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="1">
         <v>9.6175258747001793E-2</v>
       </c>
     </row>
@@ -2586,7 +2596,7 @@
       <c r="C108">
         <v>32546.285</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="1">
         <v>8.6233240458408397E-2</v>
       </c>
     </row>
@@ -2600,7 +2610,7 @@
       <c r="C109">
         <v>3957.7089999999998</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="1">
         <v>8.51182452050257E-2</v>
       </c>
     </row>
@@ -2614,7 +2624,7 @@
       <c r="C110">
         <v>9420.9069999999992</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="1">
         <v>8.3174948281110606E-2</v>
       </c>
     </row>
@@ -2628,7 +2638,7 @@
       <c r="C111">
         <v>950.64599999999996</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="1">
         <v>7.4750013170651497E-2</v>
       </c>
     </row>
@@ -2642,7 +2652,7 @@
       <c r="C112">
         <v>12707.999</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="1">
         <v>7.0932720131045804E-2</v>
       </c>
     </row>
@@ -2656,7 +2666,7 @@
       <c r="C113">
         <v>57157.271999999997</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="1">
         <v>6.7770813732146204E-2</v>
       </c>
     </row>
@@ -2670,7 +2680,7 @@
       <c r="C114">
         <v>26482.663</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="1">
         <v>6.58404152521289E-2</v>
       </c>
     </row>
@@ -2684,7 +2694,7 @@
       <c r="C115">
         <v>40644.601000000002</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="1">
         <v>4.8511204622794998E-2</v>
       </c>
     </row>
@@ -2698,7 +2708,7 @@
       <c r="C116">
         <v>26660.68</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="1">
         <v>4.4952400735878702E-2</v>
       </c>
     </row>
@@ -2712,7 +2722,7 @@
       <c r="C117">
         <v>12627.851000000001</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="1">
         <v>3.9015793673348197E-2</v>
       </c>
     </row>
@@ -2726,7 +2736,7 @@
       <c r="C118">
         <v>11092.052</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="1">
         <v>3.80688646470815E-2</v>
       </c>
     </row>
@@ -2740,7 +2750,7 @@
       <c r="C119">
         <v>13851.022999999999</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="1">
         <v>3.75259106080163E-2</v>
       </c>
     </row>
@@ -2754,7 +2764,7 @@
       <c r="C120">
         <v>29753.413</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="1">
         <v>3.5423701557439E-2</v>
       </c>
     </row>
@@ -2768,7 +2778,7 @@
       <c r="C121">
         <v>1935.0889999999999</v>
       </c>
-      <c r="D121">
+      <c r="D121" s="1">
         <v>3.5068081503534201E-2</v>
       </c>
     </row>
@@ -2782,7 +2792,7 @@
       <c r="C122">
         <v>11988.413</v>
       </c>
-      <c r="D122">
+      <c r="D122" s="1">
         <v>3.44357407925985E-2</v>
       </c>
     </row>
@@ -2796,7 +2806,7 @@
       <c r="C123">
         <v>68964.301000000007</v>
       </c>
-      <c r="D123">
+      <c r="D123" s="1">
         <v>3.2444718078793698E-2</v>
       </c>
     </row>
@@ -2810,7 +2820,7 @@
       <c r="C124">
         <v>97724.206000000006</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="1">
         <v>2.95236932047858E-2</v>
       </c>
     </row>
@@ -2824,7 +2834,7 @@
       <c r="C125">
         <v>1035.126</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="1">
         <v>2.9187855833491001E-2</v>
       </c>
     </row>
@@ -2838,7 +2848,7 @@
       <c r="C126">
         <v>1327.394</v>
       </c>
-      <c r="D126">
+      <c r="D126" s="1">
         <v>2.7483620317680101E-2</v>
       </c>
     </row>
@@ -2852,7 +2862,7 @@
       <c r="C127">
         <v>4981.8440000000001</v>
       </c>
-      <c r="D127">
+      <c r="D127" s="1">
         <v>2.7098868165263201E-2</v>
       </c>
     </row>
@@ -2866,7 +2876,7 @@
       <c r="C128">
         <v>6951.8710000000001</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="1">
         <v>2.44474783199558E-2</v>
       </c>
     </row>
@@ -2880,7 +2890,7 @@
       <c r="C129">
         <v>5050.424</v>
       </c>
-      <c r="D129">
+      <c r="D129" s="1">
         <v>2.3585508972248499E-2</v>
       </c>
     </row>
@@ -2894,7 +2904,7 @@
       <c r="C130">
         <v>32554.030999999999</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="1">
         <v>2.2307295343402801E-2</v>
       </c>
     </row>
@@ -2908,7 +2918,7 @@
       <c r="C131">
         <v>1566.3019999999999</v>
       </c>
-      <c r="D131">
+      <c r="D131" s="1">
         <v>1.89195767422011E-2</v>
       </c>
     </row>
@@ -2922,7 +2932,7 @@
       <c r="C132">
         <v>2573.9879999999998</v>
       </c>
-      <c r="D132">
+      <c r="D132" s="1">
         <v>1.7318176964739199E-2</v>
       </c>
     </row>
@@ -2936,7 +2946,7 @@
       <c r="C133">
         <v>1041.278</v>
       </c>
-      <c r="D133">
+      <c r="D133" s="1">
         <v>1.5718461952306501E-2</v>
       </c>
     </row>
@@ -2950,7 +2960,7 @@
       <c r="C134">
         <v>69161.375</v>
       </c>
-      <c r="D134">
+      <c r="D134" s="1">
         <v>1.55447094129885E-2</v>
       </c>
     </row>
@@ -2964,7 +2974,7 @@
       <c r="C135">
         <v>1939.1289999999999</v>
       </c>
-      <c r="D135">
+      <c r="D135" s="1">
         <v>1.49714153006642E-2</v>
       </c>
     </row>
@@ -2978,7 +2988,7 @@
       <c r="C136">
         <v>1395.3130000000001</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="1">
         <v>1.46295384121149E-2</v>
       </c>
     </row>
@@ -2992,7 +3002,7 @@
       <c r="C137">
         <v>130.51599999999999</v>
       </c>
-      <c r="D137">
+      <c r="D137" s="1">
         <v>1.4559303202430899E-2</v>
       </c>
     </row>
@@ -3006,7 +3016,7 @@
       <c r="C138">
         <v>2409.4699999999998</v>
       </c>
-      <c r="D138">
+      <c r="D138" s="1">
         <v>1.4390110326548199E-2</v>
       </c>
     </row>
@@ -3020,7 +3030,7 @@
       <c r="C139">
         <v>18185.876</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="1">
         <v>1.4104931118627401E-2</v>
       </c>
     </row>
@@ -3034,7 +3044,7 @@
       <c r="C140">
         <v>1229.123</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="1">
         <v>1.3737781276394899E-2</v>
       </c>
     </row>
@@ -3048,7 +3058,7 @@
       <c r="C141">
         <v>57754.27</v>
       </c>
-      <c r="D141">
+      <c r="D141" s="1">
         <v>1.34075356507525E-2</v>
       </c>
     </row>
@@ -3062,7 +3072,7 @@
       <c r="C142">
         <v>1691.567</v>
       </c>
-      <c r="D142">
+      <c r="D142" s="1">
         <v>1.28804826879159E-2</v>
       </c>
     </row>
@@ -3076,7 +3086,7 @@
       <c r="C143">
         <v>541.86500000000001</v>
       </c>
-      <c r="D143">
+      <c r="D143" s="1">
         <v>1.12368066827132E-2</v>
       </c>
     </row>
@@ -3090,7 +3100,7 @@
       <c r="C144">
         <v>63386.673999999999</v>
       </c>
-      <c r="D144">
+      <c r="D144" s="1">
         <v>1.0705902687504E-2</v>
       </c>
     </row>
@@ -3104,7 +3114,7 @@
       <c r="C145">
         <v>2721.7049999999999</v>
       </c>
-      <c r="D145">
+      <c r="D145" s="1">
         <v>1.02528401411233E-2</v>
       </c>
     </row>
@@ -3118,7 +3128,7 @@
       <c r="C146">
         <v>1145.009</v>
       </c>
-      <c r="D146">
+      <c r="D146" s="1">
         <v>1.00417073995752E-2</v>
       </c>
     </row>
@@ -3132,7 +3142,7 @@
       <c r="C147">
         <v>2978.8620000000001</v>
       </c>
-      <c r="D147">
+      <c r="D147" s="1">
         <v>9.5866741951881294E-3</v>
       </c>
     </row>
@@ -3146,7 +3156,7 @@
       <c r="C148">
         <v>1781.395</v>
       </c>
-      <c r="D148">
+      <c r="D148" s="1">
         <v>9.3120710425089893E-3</v>
       </c>
     </row>
@@ -3160,7 +3170,7 @@
       <c r="C149">
         <v>9467.51</v>
       </c>
-      <c r="D149">
+      <c r="D149" s="1">
         <v>8.6397301140064397E-3</v>
       </c>
     </row>
@@ -3174,7 +3184,7 @@
       <c r="C150">
         <v>945.44</v>
       </c>
-      <c r="D150">
+      <c r="D150" s="1">
         <v>8.4461576656000899E-3</v>
       </c>
     </row>
@@ -3188,7 +3198,7 @@
       <c r="C151">
         <v>415.01299999999998</v>
       </c>
-      <c r="D151">
+      <c r="D151" s="1">
         <v>8.2056050633522101E-3</v>
       </c>
     </row>
@@ -3202,7 +3212,7 @@
       <c r="C152">
         <v>2713.181</v>
       </c>
-      <c r="D152">
+      <c r="D152" s="1">
         <v>8.10650114452993E-3</v>
       </c>
     </row>
@@ -3216,7 +3226,7 @@
       <c r="C153">
         <v>59923.43</v>
       </c>
-      <c r="D153">
+      <c r="D153" s="1">
         <v>8.0038767533959793E-3</v>
       </c>
     </row>
@@ -3230,7 +3240,7 @@
       <c r="C154">
         <v>15.12</v>
       </c>
-      <c r="D154">
+      <c r="D154" s="1">
         <v>7.6205836399374999E-3</v>
       </c>
     </row>
@@ -3244,7 +3254,7 @@
       <c r="C155">
         <v>8.6940000000000008</v>
       </c>
-      <c r="D155">
+      <c r="D155" s="1">
         <v>7.5586197303101196E-3</v>
       </c>
     </row>
@@ -3258,7 +3268,7 @@
       <c r="C156">
         <v>1298.98</v>
       </c>
-      <c r="D156">
+      <c r="D156" s="1">
         <v>7.4224641966298696E-3</v>
       </c>
     </row>
@@ -3272,7 +3282,7 @@
       <c r="C157">
         <v>2236.9549999999999</v>
       </c>
-      <c r="D157">
+      <c r="D157" s="1">
         <v>7.1570112526029503E-3</v>
       </c>
     </row>
@@ -3286,7 +3296,7 @@
       <c r="C158">
         <v>1745.2239999999999</v>
       </c>
-      <c r="D158">
+      <c r="D158" s="1">
         <v>6.61614150280866E-3</v>
       </c>
     </row>
@@ -3300,7 +3310,7 @@
       <c r="C159">
         <v>508.21199999999999</v>
       </c>
-      <c r="D159">
+      <c r="D159" s="1">
         <v>6.3709785087975E-3</v>
       </c>
     </row>
@@ -3314,7 +3324,7 @@
       <c r="C160">
         <v>2784.6089999999999</v>
       </c>
-      <c r="D160">
+      <c r="D160" s="1">
         <v>6.3501545447847202E-3</v>
       </c>
     </row>
@@ -3328,7 +3338,7 @@
       <c r="C161">
         <v>2962.8820000000001</v>
       </c>
-      <c r="D161">
+      <c r="D161" s="1">
         <v>5.5101550455354401E-3</v>
       </c>
     </row>
@@ -3342,7 +3352,7 @@
       <c r="C162">
         <v>875.53099999999995</v>
       </c>
-      <c r="D162">
+      <c r="D162" s="1">
         <v>5.50883367302747E-3</v>
       </c>
     </row>
@@ -3356,7 +3366,7 @@
       <c r="C163">
         <v>645.12699999999995</v>
       </c>
-      <c r="D163">
+      <c r="D163" s="1">
         <v>5.3214259141853501E-3</v>
       </c>
     </row>
@@ -3370,7 +3380,7 @@
       <c r="C164">
         <v>1336.6790000000001</v>
       </c>
-      <c r="D164">
+      <c r="D164" s="1">
         <v>4.8271210243292203E-3</v>
       </c>
     </row>
@@ -3384,7 +3394,7 @@
       <c r="C165">
         <v>2624.84</v>
       </c>
-      <c r="D165">
+      <c r="D165" s="1">
         <v>4.8242049951521598E-3</v>
       </c>
     </row>
@@ -3398,7 +3408,7 @@
       <c r="C166">
         <v>801.60400000000004</v>
       </c>
-      <c r="D166">
+      <c r="D166" s="1">
         <v>4.7945773696240002E-3</v>
       </c>
     </row>
@@ -3412,7 +3422,7 @@
       <c r="C167">
         <v>2391.9630000000002</v>
       </c>
-      <c r="D167">
+      <c r="D167" s="1">
         <v>4.6654985705545599E-3</v>
       </c>
     </row>
@@ -3426,7 +3436,7 @@
       <c r="C168">
         <v>1169.0640000000001</v>
       </c>
-      <c r="D168">
+      <c r="D168" s="1">
         <v>4.5845861006174899E-3</v>
       </c>
     </row>
@@ -3440,7 +3450,7 @@
       <c r="C169">
         <v>13.023</v>
       </c>
-      <c r="D169">
+      <c r="D169" s="1">
         <v>4.23994790818818E-3</v>
       </c>
     </row>
@@ -3454,7 +3464,7 @@
       <c r="C170">
         <v>29.117000000000001</v>
       </c>
-      <c r="D170">
+      <c r="D170" s="1">
         <v>4.2390351707290103E-3</v>
       </c>
     </row>
@@ -3468,7 +3478,7 @@
       <c r="C171">
         <v>1534.7429999999999</v>
       </c>
-      <c r="D171">
+      <c r="D171" s="1">
         <v>3.9424824191711602E-3</v>
       </c>
     </row>
@@ -3482,7 +3492,7 @@
       <c r="C172">
         <v>4690.7070000000003</v>
       </c>
-      <c r="D172">
+      <c r="D172" s="1">
         <v>3.7087589850120601E-3</v>
       </c>
     </row>
@@ -3496,7 +3506,7 @@
       <c r="C173">
         <v>684.31700000000001</v>
       </c>
-      <c r="D173">
+      <c r="D173" s="1">
         <v>3.3792040367325101E-3</v>
       </c>
     </row>
@@ -3510,7 +3520,7 @@
       <c r="C174">
         <v>636.74199999999996</v>
       </c>
-      <c r="D174">
+      <c r="D174" s="1">
         <v>3.0461346780155702E-3</v>
       </c>
     </row>
@@ -3524,7 +3534,7 @@
       <c r="C175">
         <v>335.97500000000002</v>
       </c>
-      <c r="D175">
+      <c r="D175" s="1">
         <v>2.82550826560509E-3</v>
       </c>
     </row>
@@ -3538,7 +3548,7 @@
       <c r="C176">
         <v>4609.4769999999999</v>
       </c>
-      <c r="D176">
+      <c r="D176" s="1">
         <v>2.7988914136620499E-3</v>
       </c>
     </row>
@@ -3552,7 +3562,7 @@
       <c r="C177">
         <v>810.923</v>
       </c>
-      <c r="D177">
+      <c r="D177" s="1">
         <v>2.4673412874257599E-3</v>
       </c>
     </row>
@@ -3566,7 +3576,7 @@
       <c r="C178">
         <v>1020.905</v>
       </c>
-      <c r="D178">
+      <c r="D178" s="1">
         <v>2.39212139498539E-3</v>
       </c>
     </row>
@@ -3580,7 +3590,7 @@
       <c r="C179">
         <v>6099.5389999999998</v>
       </c>
-      <c r="D179">
+      <c r="D179" s="1">
         <v>2.22998619925407E-3</v>
       </c>
     </row>
@@ -3594,7 +3604,7 @@
       <c r="C180">
         <v>2223.6120000000001</v>
       </c>
-      <c r="D180">
+      <c r="D180" s="1">
         <v>2.1728880364895501E-3</v>
       </c>
     </row>
@@ -3608,7 +3618,7 @@
       <c r="C181">
         <v>915.28399999999999</v>
       </c>
-      <c r="D181">
+      <c r="D181" s="1">
         <v>2.0010144072057901E-3</v>
       </c>
     </row>
@@ -3622,7 +3632,7 @@
       <c r="C182">
         <v>2239.335</v>
       </c>
-      <c r="D182">
+      <c r="D182" s="1">
         <v>1.94786465554053E-3</v>
       </c>
     </row>
@@ -3636,7 +3646,7 @@
       <c r="C183">
         <v>293.25700000000001</v>
       </c>
-      <c r="D183">
+      <c r="D183" s="1">
         <v>1.78533737565871E-3</v>
       </c>
     </row>
@@ -3650,7 +3660,7 @@
       <c r="C184">
         <v>774.10599999999999</v>
       </c>
-      <c r="D184">
+      <c r="D184" s="1">
         <v>1.7653794867139099E-3</v>
       </c>
     </row>
@@ -3664,7 +3674,7 @@
       <c r="C185">
         <v>3737.201</v>
       </c>
-      <c r="D185">
+      <c r="D185" s="1">
         <v>1.69186543646914E-3</v>
       </c>
     </row>
@@ -3678,7 +3688,7 @@
       <c r="C186">
         <v>104.047</v>
       </c>
-      <c r="D186">
+      <c r="D186" s="1">
         <v>1.4300900164880899E-3</v>
       </c>
     </row>
@@ -3692,7 +3702,7 @@
       <c r="C187">
         <v>933.42399999999998</v>
       </c>
-      <c r="D187">
+      <c r="D187" s="1">
         <v>1.3372840891153299E-3</v>
       </c>
     </row>
@@ -3706,7 +3716,7 @@
       <c r="C188">
         <v>13887.615</v>
       </c>
-      <c r="D188">
+      <c r="D188" s="1">
         <v>1.00634571534351E-3</v>
       </c>
     </row>
@@ -3720,7 +3730,7 @@
       <c r="C189">
         <v>215.97399999999999</v>
       </c>
-      <c r="D189">
+      <c r="D189" s="1">
         <v>8.9220988823064901E-4</v>
       </c>
     </row>
@@ -3734,7 +3744,7 @@
       <c r="C190">
         <v>211.79499999999999</v>
       </c>
-      <c r="D190">
+      <c r="D190" s="1">
         <v>7.1010268635707003E-4</v>
       </c>
     </row>
@@ -3748,7 +3758,7 @@
       <c r="C191">
         <v>800.96199999999999</v>
       </c>
-      <c r="D191">
+      <c r="D191" s="1">
         <v>3.8855321855282501E-4</v>
       </c>
     </row>
@@ -3762,7 +3772,7 @@
       <c r="C192">
         <v>333.32400000000001</v>
       </c>
-      <c r="D192">
+      <c r="D192" s="1">
         <v>3.7217371000570701E-4</v>
       </c>
     </row>
@@ -3776,7 +3786,7 @@
       <c r="C193">
         <v>3399.75</v>
       </c>
-      <c r="D193">
+      <c r="D193" s="1">
         <v>2.5359949167704101E-4</v>
       </c>
     </row>
@@ -3790,7 +3800,7 @@
       <c r="C194">
         <v>19423.142</v>
       </c>
-      <c r="D194">
+      <c r="D194" s="1">
         <v>2.49180802164109E-4</v>
       </c>
     </row>
@@ -3804,7 +3814,7 @@
       <c r="C195">
         <v>47.362000000000002</v>
       </c>
-      <c r="D195">
+      <c r="D195" s="1">
         <v>1.9885983723656999E-4</v>
       </c>
     </row>
@@ -3818,7 +3828,7 @@
       <c r="C196">
         <v>8518.8809999999994</v>
       </c>
-      <c r="D196">
+      <c r="D196" s="1">
         <v>1.83602610596619E-4</v>
       </c>
     </row>
@@ -3874,7 +3884,7 @@
       <c r="C200">
         <v>0</v>
       </c>
-      <c r="D200">
+      <c r="D200" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3888,7 +3898,7 @@
       <c r="C201">
         <v>0</v>
       </c>
-      <c r="D201">
+      <c r="D201" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3902,7 +3912,7 @@
       <c r="C202">
         <v>0</v>
       </c>
-      <c r="D202">
+      <c r="D202" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3916,7 +3926,7 @@
       <c r="C203">
         <v>0</v>
       </c>
-      <c r="D203">
+      <c r="D203" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3930,7 +3940,7 @@
       <c r="C204">
         <v>0</v>
       </c>
-      <c r="D204">
+      <c r="D204" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3944,7 +3954,7 @@
       <c r="C205">
         <v>0</v>
       </c>
-      <c r="D205">
+      <c r="D205" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3958,7 +3968,7 @@
       <c r="C206">
         <v>0</v>
       </c>
-      <c r="D206">
+      <c r="D206" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3972,7 +3982,7 @@
       <c r="C207">
         <v>0</v>
       </c>
-      <c r="D207">
+      <c r="D207" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3986,7 +3996,7 @@
       <c r="C208">
         <v>0</v>
       </c>
-      <c r="D208">
+      <c r="D208" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4000,7 +4010,7 @@
       <c r="C209">
         <v>0</v>
       </c>
-      <c r="D209">
+      <c r="D209" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4014,7 +4024,7 @@
       <c r="C210">
         <v>0</v>
       </c>
-      <c r="D210">
+      <c r="D210" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4028,7 +4038,7 @@
       <c r="C211">
         <v>0</v>
       </c>
-      <c r="D211">
+      <c r="D211" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4042,7 +4052,7 @@
       <c r="C212">
         <v>0</v>
       </c>
-      <c r="D212">
+      <c r="D212" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4056,7 +4066,7 @@
       <c r="C213">
         <v>0</v>
       </c>
-      <c r="D213">
+      <c r="D213" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4070,7 +4080,7 @@
       <c r="C214">
         <v>0</v>
       </c>
-      <c r="D214">
+      <c r="D214" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4084,7 +4094,7 @@
       <c r="C215">
         <v>0</v>
       </c>
-      <c r="D215">
+      <c r="D215" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4098,7 +4108,7 @@
       <c r="C216">
         <v>0</v>
       </c>
-      <c r="D216">
+      <c r="D216" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4112,7 +4122,7 @@
       <c r="C217">
         <v>0</v>
       </c>
-      <c r="D217">
+      <c r="D217" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4126,7 +4136,7 @@
       <c r="C218">
         <v>0</v>
       </c>
-      <c r="D218">
+      <c r="D218" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4140,7 +4150,7 @@
       <c r="C219">
         <v>0</v>
       </c>
-      <c r="D219">
+      <c r="D219" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4154,7 +4164,7 @@
       <c r="C220">
         <v>0</v>
       </c>
-      <c r="D220">
+      <c r="D220" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>